<commit_message>
`Removed unused CSS files and updated relative paths in HTML files`
</commit_message>
<xml_diff>
--- a/excel/data.xlsx
+++ b/excel/data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="11">
   <si>
     <t>Name</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>amman2</t>
+  </si>
+  <si>
+    <t>fraud</t>
   </si>
 </sst>
 </file>
@@ -406,7 +409,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -480,6 +483,17 @@
         <v>7</v>
       </c>
     </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="6">
+        <v>8368547181</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>